<commit_message>
testes com ann, knn, svm
</commit_message>
<xml_diff>
--- a/Python/acc_p_value_matrix_ann.xlsx
+++ b/Python/acc_p_value_matrix_ann.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Rodrigo S. Hirama\Documentos\EACH\IC\Classification-of-mammography-images\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667A5A0B-1764-4B4E-B357-D67D02F1718A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF6AB88-4F1B-454E-8960-EBBCCCEFE289}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -364,7 +364,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -439,61 +439,61 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.26327996688233513</v>
+        <v>0.52559724276333442</v>
       </c>
       <c r="D2">
-        <v>0.86162778737753887</v>
+        <v>0.78424387949001195</v>
       </c>
       <c r="E2">
-        <v>4.3210332003537251E-2</v>
+        <v>3.3221010230918391E-2</v>
       </c>
       <c r="F2">
-        <v>5.025264943939918E-2</v>
+        <v>2.588505231274273E-2</v>
       </c>
       <c r="G2">
-        <v>2.4341545208082611E-3</v>
+        <v>2.6091417323220831E-4</v>
       </c>
       <c r="H2">
-        <v>0.8993420133543466</v>
+        <v>0.85812799862225753</v>
       </c>
       <c r="I2">
-        <v>0.19811684524496359</v>
+        <v>0.10792468896806499</v>
       </c>
       <c r="J2">
-        <v>0.57023988173522677</v>
+        <v>0.95094071278253867</v>
       </c>
       <c r="K2">
-        <v>0.79839635497623374</v>
+        <v>0.90388208304665207</v>
       </c>
       <c r="L2">
-        <v>0.57178496411042956</v>
+        <v>0.85607569409172035</v>
       </c>
       <c r="M2">
-        <v>0.17840782082983711</v>
+        <v>8.6726284033961848E-2</v>
       </c>
       <c r="N2">
-        <v>0.62293967943553885</v>
+        <v>0.47051471586977872</v>
       </c>
       <c r="O2">
-        <v>0.25951959673663888</v>
+        <v>0.62229974261625232</v>
       </c>
       <c r="P2">
-        <v>0.14061720441686329</v>
+        <v>0.28842691791756042</v>
       </c>
       <c r="Q2">
-        <v>0.12989389742245341</v>
+        <v>0.28500787755524792</v>
       </c>
       <c r="R2">
-        <v>2.1789919836982089E-4</v>
+        <v>1.4136308980620159E-3</v>
       </c>
       <c r="S2">
-        <v>2.7845022154248019E-5</v>
+        <v>1.7102037483970849E-5</v>
       </c>
       <c r="T2">
-        <v>1.457696625829247E-3</v>
+        <v>1.5270157393455291E-3</v>
       </c>
       <c r="U2">
-        <v>5.2839601324109701E-3</v>
+        <v>6.6736722316070498E-3</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -501,64 +501,64 @@
         <v>2E-3</v>
       </c>
       <c r="B3">
-        <v>0.26327996688233513</v>
+        <v>0.52559724276333442</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.38175993510436468</v>
+        <v>0.74252405734647842</v>
       </c>
       <c r="E3">
-        <v>1.6189776902270981E-3</v>
+        <v>0.13807270777435179</v>
       </c>
       <c r="F3">
-        <v>2.0091420019272498E-3</v>
+        <v>0.1163224214423476</v>
       </c>
       <c r="G3">
-        <v>2.700133335224216E-5</v>
+        <v>2.9253375170850159E-3</v>
       </c>
       <c r="H3">
-        <v>0.30958779519213142</v>
+        <v>0.63369929622892962</v>
       </c>
       <c r="I3">
-        <v>1.446824469671565E-2</v>
+        <v>0.35268685426591118</v>
       </c>
       <c r="J3">
-        <v>0.56817466041076847</v>
+        <v>0.53861771023598193</v>
       </c>
       <c r="K3">
-        <v>0.36915814135330532</v>
+        <v>0.43288550438411849</v>
       </c>
       <c r="L3">
-        <v>0.56974192998939011</v>
+        <v>0.39777961290617841</v>
       </c>
       <c r="M3">
-        <v>1.2458031467910699E-2</v>
+        <v>0.28663756342887731</v>
       </c>
       <c r="N3">
-        <v>0.1092875435142603</v>
+        <v>0.95201970184889118</v>
       </c>
       <c r="O3">
-        <v>0.99999999999999445</v>
+        <v>0.24275148431932941</v>
       </c>
       <c r="P3">
-        <v>0.71048148464631267</v>
+        <v>8.7950970922562086E-2</v>
       </c>
       <c r="Q3">
-        <v>0.70267583579861115</v>
+        <v>8.5724029343540148E-2</v>
       </c>
       <c r="R3">
-        <v>7.4560962411704531E-3</v>
+        <v>1.3338649853724289E-4</v>
       </c>
       <c r="S3">
-        <v>1.5826331585101429E-3</v>
+        <v>1.06107141825917E-6</v>
       </c>
       <c r="T3">
-        <v>3.510314829876366E-2</v>
+        <v>1.4844154560446441E-4</v>
       </c>
       <c r="U3">
-        <v>9.5350640566264244E-2</v>
+        <v>8.2364487698628253E-4</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -566,64 +566,64 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="B4">
-        <v>0.86162778737753887</v>
+        <v>0.78424387949001195</v>
       </c>
       <c r="C4">
-        <v>0.38175993510436468</v>
+        <v>0.74252405734647842</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>3.8660260073889438E-2</v>
+        <v>8.2355609179215E-2</v>
       </c>
       <c r="F4">
-        <v>4.462822354464404E-2</v>
+        <v>6.8429330847235306E-2</v>
       </c>
       <c r="G4">
-        <v>2.6826913135310619E-3</v>
+        <v>1.6744394417949129E-3</v>
       </c>
       <c r="H4">
-        <v>0.95280136557354445</v>
+        <v>0.91029381276574473</v>
       </c>
       <c r="I4">
-        <v>0.16721732865082409</v>
+        <v>0.2210246894391632</v>
       </c>
       <c r="J4">
-        <v>0.72306080590456112</v>
+        <v>0.81666362891201971</v>
       </c>
       <c r="K4">
-        <v>0.95240163110510501</v>
+        <v>0.68993758541312677</v>
       </c>
       <c r="L4">
-        <v>0.72399407467518739</v>
+        <v>0.64807629061215422</v>
       </c>
       <c r="M4">
-        <v>0.15100245539659471</v>
+        <v>0.179324023412511</v>
       </c>
       <c r="N4">
-        <v>0.52559724276330866</v>
+        <v>0.6908233002137828</v>
       </c>
       <c r="O4">
-        <v>0.37845625746999129</v>
+        <v>0.45102021260479452</v>
       </c>
       <c r="P4">
-        <v>0.2256584700698708</v>
+        <v>0.19957590605155301</v>
       </c>
       <c r="Q4">
-        <v>0.21450884488791419</v>
+        <v>0.19673172269215011</v>
       </c>
       <c r="R4">
-        <v>8.7235605196196221E-4</v>
+        <v>9.9288215984399508E-4</v>
       </c>
       <c r="S4">
-        <v>1.5433898983535529E-4</v>
+        <v>1.392113014431501E-5</v>
       </c>
       <c r="T4">
-        <v>4.7798366882050164E-3</v>
+        <v>1.068054240261916E-3</v>
       </c>
       <c r="U4">
-        <v>1.492075737143009E-2</v>
+        <v>4.4959054682820734E-3</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -631,64 +631,64 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="B5">
-        <v>4.3210332003537251E-2</v>
+        <v>3.3221010230918391E-2</v>
       </c>
       <c r="C5">
-        <v>1.6189776902270981E-3</v>
+        <v>0.13807270777435179</v>
       </c>
       <c r="D5">
-        <v>3.8660260073889438E-2</v>
+        <v>8.2355609179215E-2</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.94804330363837341</v>
+        <v>0.95006114650670237</v>
       </c>
       <c r="G5">
-        <v>0.33702478570806288</v>
+        <v>0.14486716311853659</v>
       </c>
       <c r="H5">
-        <v>2.82178073156499E-2</v>
+        <v>4.3411853614882902E-2</v>
       </c>
       <c r="I5">
-        <v>0.42684750904426177</v>
+        <v>0.52094271258660907</v>
       </c>
       <c r="J5">
-        <v>8.4746533842678662E-3</v>
+        <v>2.6808168888947981E-2</v>
       </c>
       <c r="K5">
-        <v>1.902468490752986E-2</v>
+        <v>1.8554377358978941E-2</v>
       </c>
       <c r="L5">
-        <v>8.7511241058760136E-3</v>
+        <v>1.5573279997438931E-2</v>
       </c>
       <c r="M5">
-        <v>0.4681846601227363</v>
+        <v>0.6684885640234155</v>
       </c>
       <c r="N5">
-        <v>0.1315012434037727</v>
+        <v>0.1367829850551176</v>
       </c>
       <c r="O5">
-        <v>1.482115381740911E-3</v>
+        <v>5.4860888808857646E-3</v>
       </c>
       <c r="P5">
-        <v>5.0067097688034966E-4</v>
+        <v>1.1662127256724191E-3</v>
       </c>
       <c r="Q5">
-        <v>3.4382049796309383E-4</v>
+        <v>1.07143407053676E-3</v>
       </c>
       <c r="R5">
-        <v>2.4050491340163989E-8</v>
+        <v>8.1264830760232808E-8</v>
       </c>
       <c r="S5">
-        <v>1.0558934461814369E-9</v>
+        <v>2.6247470567174799E-10</v>
       </c>
       <c r="T5">
-        <v>2.4384086860006531E-7</v>
+        <v>1.003731476134684E-7</v>
       </c>
       <c r="U5">
-        <v>1.232362978881478E-6</v>
+        <v>1.0211313050519151E-6</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -696,64 +696,64 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="B6">
-        <v>5.025264943939918E-2</v>
+        <v>2.588505231274273E-2</v>
       </c>
       <c r="C6">
-        <v>2.0091420019272498E-3</v>
+        <v>0.1163224214423476</v>
       </c>
       <c r="D6">
-        <v>4.462822354464404E-2</v>
+        <v>6.8429330847235306E-2</v>
       </c>
       <c r="E6">
-        <v>0.94804330363837341</v>
+        <v>0.95006114650670237</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.30411347575479097</v>
+        <v>0.15437766746700429</v>
       </c>
       <c r="H6">
-        <v>3.3256529777094278E-2</v>
+        <v>3.3908643731070193E-2</v>
       </c>
       <c r="I6">
-        <v>0.466649750301525</v>
+        <v>0.470714067831139</v>
       </c>
       <c r="J6">
-        <v>1.0239186113398231E-2</v>
+        <v>2.0090267956356971E-2</v>
       </c>
       <c r="K6">
-        <v>2.2658039689091861E-2</v>
+        <v>1.373561047019998E-2</v>
       </c>
       <c r="L6">
-        <v>1.0558010794286679E-2</v>
+        <v>1.140885655833911E-2</v>
       </c>
       <c r="M6">
-        <v>0.50984154535829673</v>
+        <v>0.61779658736411025</v>
       </c>
       <c r="N6">
-        <v>0.148527820606595</v>
+        <v>0.1139288340030714</v>
       </c>
       <c r="O6">
-        <v>1.845401858084053E-3</v>
+        <v>3.7518954869757691E-3</v>
       </c>
       <c r="P6">
-        <v>6.3115988963810998E-4</v>
+        <v>7.5671999185642142E-4</v>
       </c>
       <c r="Q6">
-        <v>4.3896521475213321E-4</v>
+        <v>6.8868663855314253E-4</v>
       </c>
       <c r="R6">
-        <v>3.3437872633855629E-8</v>
+        <v>3.3772957366291222E-8</v>
       </c>
       <c r="S6">
-        <v>1.5173244844381209E-9</v>
+        <v>9.5239168603861024E-11</v>
       </c>
       <c r="T6">
-        <v>3.3681775712912058E-7</v>
+        <v>4.2560440834142919E-8</v>
       </c>
       <c r="U6">
-        <v>1.694081506672887E-6</v>
+        <v>4.7622304855678139E-7</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -761,64 +761,64 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="B7">
-        <v>2.4341545208082611E-3</v>
+        <v>2.6091417323220831E-4</v>
       </c>
       <c r="C7">
-        <v>2.700133335224216E-5</v>
+        <v>2.9253375170850159E-3</v>
       </c>
       <c r="D7">
-        <v>2.6826913135310619E-3</v>
+        <v>1.6744394417949129E-3</v>
       </c>
       <c r="E7">
-        <v>0.33702478570806288</v>
+        <v>0.14486716311853659</v>
       </c>
       <c r="F7">
-        <v>0.30411347575479097</v>
+        <v>0.15437766746700429</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>1.210105721386243E-3</v>
+        <v>3.1567194178821708E-4</v>
       </c>
       <c r="I7">
-        <v>7.0337348693443352E-2</v>
+        <v>2.5917065330912571E-2</v>
       </c>
       <c r="J7">
-        <v>2.2960509311625239E-4</v>
+        <v>1.060520603838103E-4</v>
       </c>
       <c r="K7">
-        <v>6.622720743616659E-4</v>
+        <v>6.8784303944808759E-5</v>
       </c>
       <c r="L7">
-        <v>2.4506192323812601E-4</v>
+        <v>5.1097277120532239E-5</v>
       </c>
       <c r="M7">
-        <v>8.3158139732835631E-2</v>
+        <v>5.6152165695731122E-2</v>
       </c>
       <c r="N7">
-        <v>1.2677309160734271E-2</v>
+        <v>2.1845283884574891E-3</v>
       </c>
       <c r="O7">
-        <v>2.290999675423765E-5</v>
+        <v>7.958975996170917E-6</v>
       </c>
       <c r="P7">
-        <v>6.2885212039726953E-6</v>
+        <v>1.197927279515547E-6</v>
       </c>
       <c r="Q7">
-        <v>3.2230343808722132E-6</v>
+        <v>9.7466557416368469E-7</v>
       </c>
       <c r="R7">
-        <v>4.3955822418248478E-11</v>
+        <v>1.9539623387759358E-12</v>
       </c>
       <c r="S7">
-        <v>9.0292433946878349E-13</v>
+        <v>3.30014080024919E-15</v>
       </c>
       <c r="T7">
-        <v>4.8043364493501045E-10</v>
+        <v>2.9135386384554079E-12</v>
       </c>
       <c r="U7">
-        <v>2.5293896648204482E-9</v>
+        <v>5.9786755238398405E-11</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -826,64 +826,64 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="B8">
-        <v>0.8993420133543466</v>
+        <v>0.85812799862225753</v>
       </c>
       <c r="C8">
-        <v>0.30958779519213142</v>
+        <v>0.63369929622892962</v>
       </c>
       <c r="D8">
-        <v>0.95280136557354445</v>
+        <v>0.91029381276574473</v>
       </c>
       <c r="E8">
-        <v>2.82178073156499E-2</v>
+        <v>4.3411853614882902E-2</v>
       </c>
       <c r="F8">
-        <v>3.3256529777094278E-2</v>
+        <v>3.3908643731070193E-2</v>
       </c>
       <c r="G8">
-        <v>1.210105721386243E-3</v>
+        <v>3.1567194178821708E-4</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>0.14771794813619329</v>
+        <v>0.1399809223181771</v>
       </c>
       <c r="J8">
-        <v>0.65170192921352887</v>
+        <v>0.89850015672725692</v>
       </c>
       <c r="K8">
-        <v>0.89607480443710363</v>
+        <v>0.75466603824611067</v>
       </c>
       <c r="L8">
-        <v>0.65306366746813627</v>
+        <v>0.70728971553951103</v>
       </c>
       <c r="M8">
-        <v>0.13185122352879891</v>
+        <v>0.1121555942335842</v>
       </c>
       <c r="N8">
-        <v>0.53039656415745995</v>
+        <v>0.57527664562901981</v>
       </c>
       <c r="O8">
-        <v>0.30560398022463359</v>
+        <v>0.48270346465542291</v>
       </c>
       <c r="P8">
-        <v>0.16770116573373789</v>
+        <v>0.2007899310092616</v>
       </c>
       <c r="Q8">
-        <v>0.15567336535874171</v>
+        <v>0.19738777347817929</v>
       </c>
       <c r="R8">
-        <v>2.5989928872761708E-4</v>
+        <v>5.0655873098462705E-4</v>
       </c>
       <c r="S8">
-        <v>3.2254242963141942E-5</v>
+        <v>4.3884573994100568E-6</v>
       </c>
       <c r="T8">
-        <v>1.763703066628202E-3</v>
+        <v>5.5781136854532898E-4</v>
       </c>
       <c r="U8">
-        <v>6.4407239952002414E-3</v>
+        <v>2.8590671473384252E-3</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -891,64 +891,64 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="B9">
-        <v>0.19811684524496359</v>
+        <v>0.10792468896806499</v>
       </c>
       <c r="C9">
-        <v>1.446824469671565E-2</v>
+        <v>0.35268685426591118</v>
       </c>
       <c r="D9">
-        <v>0.16721732865082409</v>
+        <v>0.2210246894391632</v>
       </c>
       <c r="E9">
-        <v>0.42684750904426177</v>
+        <v>0.52094271258660907</v>
       </c>
       <c r="F9">
-        <v>0.466649750301525</v>
+        <v>0.470714067831139</v>
       </c>
       <c r="G9">
-        <v>7.0337348693443352E-2</v>
+        <v>2.5917065330912571E-2</v>
       </c>
       <c r="H9">
-        <v>0.14771794813619329</v>
+        <v>0.1399809223181771</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>5.7450750021117512E-2</v>
+        <v>9.6058173183336037E-2</v>
       </c>
       <c r="K9">
-        <v>0.1107065533342335</v>
+        <v>6.8453780226291713E-2</v>
       </c>
       <c r="L9">
-        <v>5.8536074119757968E-2</v>
+        <v>5.8840457070609357E-2</v>
       </c>
       <c r="M9">
-        <v>0.94650998486587989</v>
+        <v>0.84783035227994774</v>
       </c>
       <c r="N9">
-        <v>0.44298807136438739</v>
+        <v>0.36267964811914222</v>
       </c>
       <c r="O9">
-        <v>1.365561890233649E-2</v>
+        <v>2.3844895351246041E-2</v>
       </c>
       <c r="P9">
-        <v>5.2469897071676626E-3</v>
+        <v>5.5239804766496819E-3</v>
       </c>
       <c r="Q9">
-        <v>4.0441085834885121E-3</v>
+        <v>5.1515413470594306E-3</v>
       </c>
       <c r="R9">
-        <v>6.198439090058077E-7</v>
+        <v>5.3539775809162536E-7</v>
       </c>
       <c r="S9">
-        <v>3.5372785822630202E-8</v>
+        <v>1.648638884737745E-9</v>
       </c>
       <c r="T9">
-        <v>5.9305609752617586E-6</v>
+        <v>6.5680099517370794E-7</v>
       </c>
       <c r="U9">
-        <v>2.8607680003255519E-5</v>
+        <v>6.5242895106731733E-6</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -956,64 +956,64 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="B10">
-        <v>0.57023988173522677</v>
+        <v>0.95094071278253867</v>
       </c>
       <c r="C10">
-        <v>0.56817466041076847</v>
+        <v>0.53861771023598193</v>
       </c>
       <c r="D10">
-        <v>0.72306080590456112</v>
+        <v>0.81666362891201971</v>
       </c>
       <c r="E10">
-        <v>8.4746533842678662E-3</v>
+        <v>2.6808168888947981E-2</v>
       </c>
       <c r="F10">
-        <v>1.0239186113398231E-2</v>
+        <v>2.0090267956356971E-2</v>
       </c>
       <c r="G10">
-        <v>2.2960509311625239E-4</v>
+        <v>1.060520603838103E-4</v>
       </c>
       <c r="H10">
-        <v>0.65170192921352887</v>
+        <v>0.89850015672725692</v>
       </c>
       <c r="I10">
-        <v>5.7450750021117512E-2</v>
+        <v>9.6058173183336037E-2</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0.74463413204514739</v>
+        <v>0.84597871090243504</v>
       </c>
       <c r="L10">
-        <v>0.99999999999999434</v>
+        <v>0.79533895606583394</v>
       </c>
       <c r="M10">
-        <v>5.0378345113161013E-2</v>
+        <v>7.6986030745351111E-2</v>
       </c>
       <c r="N10">
-        <v>0.28769457435511409</v>
+        <v>0.4782791519866334</v>
       </c>
       <c r="O10">
-        <v>0.56498832068917559</v>
+        <v>0.5511502420708293</v>
       </c>
       <c r="P10">
-        <v>0.34734592903007699</v>
+        <v>0.23116307250736801</v>
       </c>
       <c r="Q10">
-        <v>0.33352367304492841</v>
+        <v>0.22738711370285669</v>
       </c>
       <c r="R10">
-        <v>1.203136736078733E-3</v>
+        <v>5.1324067860262969E-4</v>
       </c>
       <c r="S10">
-        <v>1.8654524256988891E-4</v>
+        <v>3.869742778490119E-6</v>
       </c>
       <c r="T10">
-        <v>7.1008947164402916E-3</v>
+        <v>5.6892603831093025E-4</v>
       </c>
       <c r="U10">
-        <v>2.3125072238761819E-2</v>
+        <v>3.067918144626237E-3</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -1021,64 +1021,64 @@
         <v>0.01</v>
       </c>
       <c r="B11">
-        <v>0.79839635497623374</v>
+        <v>0.90388208304665207</v>
       </c>
       <c r="C11">
-        <v>0.36915814135330532</v>
+        <v>0.43288550438411849</v>
       </c>
       <c r="D11">
-        <v>0.95240163110510501</v>
+        <v>0.68993758541312677</v>
       </c>
       <c r="E11">
-        <v>1.902468490752986E-2</v>
+        <v>1.8554377358978941E-2</v>
       </c>
       <c r="F11">
-        <v>2.2658039689091861E-2</v>
+        <v>1.373561047019998E-2</v>
       </c>
       <c r="G11">
-        <v>6.622720743616659E-4</v>
+        <v>6.8784303944808759E-5</v>
       </c>
       <c r="H11">
-        <v>0.89607480443710363</v>
+        <v>0.75466603824611067</v>
       </c>
       <c r="I11">
-        <v>0.1107065533342335</v>
+        <v>6.8453780226291713E-2</v>
       </c>
       <c r="J11">
-        <v>0.74463413204514739</v>
+        <v>0.84597871090243504</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>0.7456867654683963</v>
+        <v>0.94935712630640701</v>
       </c>
       <c r="M11">
-        <v>9.8115495748855266E-2</v>
+        <v>5.5118891147690093E-2</v>
       </c>
       <c r="N11">
-        <v>0.44731708052311853</v>
+        <v>0.37684065098303499</v>
       </c>
       <c r="O11">
-        <v>0.36513151983949221</v>
+        <v>0.69733624316937926</v>
       </c>
       <c r="P11">
-        <v>0.20526189564235919</v>
+        <v>0.32259165217491093</v>
       </c>
       <c r="Q11">
-        <v>0.19211997075003101</v>
+        <v>0.31881657082178388</v>
       </c>
       <c r="R11">
-        <v>3.609633144474376E-4</v>
+        <v>1.260346703722178E-3</v>
       </c>
       <c r="S11">
-        <v>4.5750780011298987E-5</v>
+        <v>1.230131765060612E-5</v>
       </c>
       <c r="T11">
-        <v>2.4156140948717532E-3</v>
+        <v>1.3741641335705029E-3</v>
       </c>
       <c r="U11">
-        <v>8.7024165045004372E-3</v>
+        <v>6.5011712523409051E-3</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -1086,64 +1086,64 @@
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="B12">
-        <v>0.57178496411042956</v>
+        <v>0.85607569409172035</v>
       </c>
       <c r="C12">
-        <v>0.56974192998939011</v>
+        <v>0.39777961290617841</v>
       </c>
       <c r="D12">
-        <v>0.72399407467518739</v>
+        <v>0.64807629061215422</v>
       </c>
       <c r="E12">
-        <v>8.7511241058760136E-3</v>
+        <v>1.5573279997438931E-2</v>
       </c>
       <c r="F12">
-        <v>1.0558010794286679E-2</v>
+        <v>1.140885655833911E-2</v>
       </c>
       <c r="G12">
-        <v>2.4506192323812601E-4</v>
+        <v>5.1097277120532239E-5</v>
       </c>
       <c r="H12">
-        <v>0.65306366746813627</v>
+        <v>0.70728971553951103</v>
       </c>
       <c r="I12">
-        <v>5.8536074119757968E-2</v>
+        <v>5.8840457070609357E-2</v>
       </c>
       <c r="J12">
-        <v>0.99999999999999434</v>
+        <v>0.79533895606583394</v>
       </c>
       <c r="K12">
-        <v>0.7456867654683963</v>
+        <v>0.94935712630640701</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>5.1371725038777537E-2</v>
+        <v>4.7486580048028422E-2</v>
       </c>
       <c r="N12">
-        <v>0.28959686497139969</v>
+        <v>0.34309044002841271</v>
       </c>
       <c r="O12">
-        <v>0.56659022851237484</v>
+        <v>0.74547727961561572</v>
       </c>
       <c r="P12">
-        <v>0.34925430667919988</v>
+        <v>0.35302351905773061</v>
       </c>
       <c r="Q12">
-        <v>0.33554949906542031</v>
+        <v>0.34925430667919921</v>
       </c>
       <c r="R12">
-        <v>1.2535561191343481E-3</v>
+        <v>1.530740753559435E-3</v>
       </c>
       <c r="S12">
-        <v>1.9729909762036189E-4</v>
+        <v>1.5472191632818931E-5</v>
       </c>
       <c r="T12">
-        <v>7.3303458719044179E-3</v>
+        <v>1.664861959675016E-3</v>
       </c>
       <c r="U12">
-        <v>2.371371235314473E-2</v>
+        <v>7.7149012146084774E-3</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
@@ -1151,64 +1151,64 @@
         <v>1.2E-2</v>
       </c>
       <c r="B13">
-        <v>0.17840782082983711</v>
+        <v>8.6726284033961848E-2</v>
       </c>
       <c r="C13">
-        <v>1.2458031467910699E-2</v>
+        <v>0.28663756342887731</v>
       </c>
       <c r="D13">
-        <v>0.15100245539659471</v>
+        <v>0.179324023412511</v>
       </c>
       <c r="E13">
-        <v>0.4681846601227363</v>
+        <v>0.6684885640234155</v>
       </c>
       <c r="F13">
-        <v>0.50984154535829673</v>
+        <v>0.61779658736411025</v>
       </c>
       <c r="G13">
-        <v>8.3158139732835631E-2</v>
+        <v>5.6152165695731122E-2</v>
       </c>
       <c r="H13">
-        <v>0.13185122352879891</v>
+        <v>0.1121555942335842</v>
       </c>
       <c r="I13">
-        <v>0.94650998486587989</v>
+        <v>0.84783035227994774</v>
       </c>
       <c r="J13">
-        <v>5.0378345113161013E-2</v>
+        <v>7.6986030745351111E-2</v>
       </c>
       <c r="K13">
-        <v>9.8115495748855266E-2</v>
+        <v>5.5118891147690093E-2</v>
       </c>
       <c r="L13">
-        <v>5.1371725038777537E-2</v>
+        <v>4.7486580048028422E-2</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
-        <v>0.40781246258924059</v>
+        <v>0.29306063126893672</v>
       </c>
       <c r="O13">
-        <v>1.1737472035450161E-2</v>
+        <v>1.966237411548127E-2</v>
       </c>
       <c r="P13">
-        <v>4.4731431019285617E-3</v>
+        <v>4.7262834179107689E-3</v>
       </c>
       <c r="Q13">
-        <v>3.4255609968250741E-3</v>
+        <v>4.42685358102121E-3</v>
       </c>
       <c r="R13">
-        <v>5.060755225612102E-7</v>
+        <v>7.2087879131648591E-7</v>
       </c>
       <c r="S13">
-        <v>2.867621090557356E-8</v>
+        <v>2.787233900006273E-9</v>
       </c>
       <c r="T13">
-        <v>4.8478256205278986E-6</v>
+        <v>8.6450831582886772E-7</v>
       </c>
       <c r="U13">
-        <v>2.3418433924893479E-5</v>
+        <v>7.6034113311076567E-6</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
@@ -1216,64 +1216,64 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="B14">
-        <v>0.62293967943553885</v>
+        <v>0.47051471586977872</v>
       </c>
       <c r="C14">
-        <v>0.1092875435142603</v>
+        <v>0.95201970184889118</v>
       </c>
       <c r="D14">
-        <v>0.52559724276330866</v>
+        <v>0.6908233002137828</v>
       </c>
       <c r="E14">
-        <v>0.1315012434037727</v>
+        <v>0.1367829850551176</v>
       </c>
       <c r="F14">
-        <v>0.148527820606595</v>
+        <v>0.1139288340030714</v>
       </c>
       <c r="G14">
-        <v>1.2677309160734271E-2</v>
+        <v>2.1845283884574891E-3</v>
       </c>
       <c r="H14">
-        <v>0.53039656415745995</v>
+        <v>0.57527664562901981</v>
       </c>
       <c r="I14">
-        <v>0.44298807136438739</v>
+        <v>0.36267964811914222</v>
       </c>
       <c r="J14">
-        <v>0.28769457435511409</v>
+        <v>0.4782791519866334</v>
       </c>
       <c r="K14">
-        <v>0.44731708052311853</v>
+        <v>0.37684065098303499</v>
       </c>
       <c r="L14">
-        <v>0.28959686497139969</v>
+        <v>0.34309044002841271</v>
       </c>
       <c r="M14">
-        <v>0.40781246258924059</v>
+        <v>0.29306063126893672</v>
       </c>
       <c r="N14">
         <v>1</v>
       </c>
       <c r="O14">
-        <v>0.1065596395631692</v>
+        <v>0.19743902053378351</v>
       </c>
       <c r="P14">
-        <v>5.1578241500625718E-2</v>
+        <v>6.5414796886754056E-2</v>
       </c>
       <c r="Q14">
-        <v>4.5521395752079037E-2</v>
+        <v>6.336093586561875E-2</v>
       </c>
       <c r="R14">
-        <v>3.7681179139172131E-5</v>
+        <v>5.187049399715414E-5</v>
       </c>
       <c r="S14">
-        <v>3.9468616145474359E-6</v>
+        <v>2.9946453924039251E-7</v>
       </c>
       <c r="T14">
-        <v>2.8139400653773121E-4</v>
+        <v>5.9057122000836537E-5</v>
       </c>
       <c r="U14">
-        <v>1.117803377350084E-3</v>
+        <v>3.8426256415280961E-4</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
@@ -1281,64 +1281,64 @@
         <v>1.4E-2</v>
       </c>
       <c r="B15">
-        <v>0.25951959673663888</v>
+        <v>0.62229974261625232</v>
       </c>
       <c r="C15">
-        <v>0.99999999999999445</v>
+        <v>0.24275148431932941</v>
       </c>
       <c r="D15">
-        <v>0.37845625746999129</v>
+        <v>0.45102021260479452</v>
       </c>
       <c r="E15">
-        <v>1.482115381740911E-3</v>
+        <v>5.4860888808857646E-3</v>
       </c>
       <c r="F15">
-        <v>1.845401858084053E-3</v>
+        <v>3.7518954869757691E-3</v>
       </c>
       <c r="G15">
-        <v>2.290999675423765E-5</v>
+        <v>7.958975996170917E-6</v>
       </c>
       <c r="H15">
-        <v>0.30560398022463359</v>
+        <v>0.48270346465542291</v>
       </c>
       <c r="I15">
-        <v>1.365561890233649E-2</v>
+        <v>2.3844895351246041E-2</v>
       </c>
       <c r="J15">
-        <v>0.56498832068917559</v>
+        <v>0.5511502420708293</v>
       </c>
       <c r="K15">
-        <v>0.36513151983949221</v>
+        <v>0.69733624316937926</v>
       </c>
       <c r="L15">
-        <v>0.56659022851237484</v>
+        <v>0.74547727961561572</v>
       </c>
       <c r="M15">
-        <v>1.1737472035450161E-2</v>
+        <v>1.966237411548127E-2</v>
       </c>
       <c r="N15">
-        <v>0.1065596395631692</v>
+        <v>0.19743902053378351</v>
       </c>
       <c r="O15">
         <v>1</v>
       </c>
       <c r="P15">
-        <v>0.70831420303807646</v>
+        <v>0.5275521646949678</v>
       </c>
       <c r="Q15">
-        <v>0.70032722639946254</v>
+        <v>0.52417935966029816</v>
       </c>
       <c r="R15">
-        <v>7.0361876474006636E-3</v>
+        <v>3.4789807213629008E-3</v>
       </c>
       <c r="S15">
-        <v>1.4576966258291451E-3</v>
+        <v>3.9052448377526308E-5</v>
       </c>
       <c r="T15">
-        <v>3.3690806688296292E-2</v>
+        <v>3.7517584822295241E-3</v>
       </c>
       <c r="U15">
-        <v>9.2588237506403381E-2</v>
+        <v>1.6137422471564619E-2</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
@@ -1346,64 +1346,64 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="B16">
-        <v>0.14061720441686329</v>
+        <v>0.28842691791756042</v>
       </c>
       <c r="C16">
-        <v>0.71048148464631267</v>
+        <v>8.7950970922562086E-2</v>
       </c>
       <c r="D16">
-        <v>0.2256584700698708</v>
+        <v>0.19957590605155301</v>
       </c>
       <c r="E16">
-        <v>5.0067097688034966E-4</v>
+        <v>1.1662127256724191E-3</v>
       </c>
       <c r="F16">
-        <v>6.3115988963810998E-4</v>
+        <v>7.5671999185642142E-4</v>
       </c>
       <c r="G16">
-        <v>6.2885212039726953E-6</v>
+        <v>1.197927279515547E-6</v>
       </c>
       <c r="H16">
-        <v>0.16770116573373789</v>
+        <v>0.2007899310092616</v>
       </c>
       <c r="I16">
-        <v>5.2469897071676626E-3</v>
+        <v>5.5239804766496819E-3</v>
       </c>
       <c r="J16">
-        <v>0.34734592903007699</v>
+        <v>0.23116307250736801</v>
       </c>
       <c r="K16">
-        <v>0.20526189564235919</v>
+        <v>0.32259165217491093</v>
       </c>
       <c r="L16">
-        <v>0.34925430667919988</v>
+        <v>0.35302351905773061</v>
       </c>
       <c r="M16">
-        <v>4.4731431019285617E-3</v>
+        <v>4.7262834179107689E-3</v>
       </c>
       <c r="N16">
-        <v>5.1578241500625718E-2</v>
+        <v>6.5414796886754056E-2</v>
       </c>
       <c r="O16">
-        <v>0.70831420303807646</v>
+        <v>0.5275521646949678</v>
       </c>
       <c r="P16">
         <v>1</v>
       </c>
       <c r="Q16">
-        <v>1</v>
+        <v>0.99999999999998812</v>
       </c>
       <c r="R16">
-        <v>2.1403128583635481E-2</v>
+        <v>2.8133102674398051E-2</v>
       </c>
       <c r="S16">
-        <v>5.5588214737046938E-3</v>
+        <v>6.7728173313055795E-4</v>
       </c>
       <c r="T16">
-        <v>8.5526783091267961E-2</v>
+        <v>2.93262762513492E-2</v>
       </c>
       <c r="U16">
-        <v>0.2041556871143243</v>
+        <v>8.891860034689382E-2</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
@@ -1411,64 +1411,64 @@
         <v>1.6E-2</v>
       </c>
       <c r="B17">
-        <v>0.12989389742245341</v>
+        <v>0.28500787755524792</v>
       </c>
       <c r="C17">
-        <v>0.70267583579861115</v>
+        <v>8.5724029343540148E-2</v>
       </c>
       <c r="D17">
-        <v>0.21450884488791419</v>
+        <v>0.19673172269215011</v>
       </c>
       <c r="E17">
-        <v>3.4382049796309383E-4</v>
+        <v>1.07143407053676E-3</v>
       </c>
       <c r="F17">
-        <v>4.3896521475213321E-4</v>
+        <v>6.8868663855314253E-4</v>
       </c>
       <c r="G17">
-        <v>3.2230343808722132E-6</v>
+        <v>9.7466557416368469E-7</v>
       </c>
       <c r="H17">
-        <v>0.15567336535874171</v>
+        <v>0.19738777347817929</v>
       </c>
       <c r="I17">
-        <v>4.0441085834885121E-3</v>
+        <v>5.1515413470594306E-3</v>
       </c>
       <c r="J17">
-        <v>0.33352367304492841</v>
+        <v>0.22738711370285669</v>
       </c>
       <c r="K17">
-        <v>0.19211997075003101</v>
+        <v>0.31881657082178388</v>
       </c>
       <c r="L17">
-        <v>0.33554949906542031</v>
+        <v>0.34925430667919921</v>
       </c>
       <c r="M17">
-        <v>3.4255609968250741E-3</v>
+        <v>4.42685358102121E-3</v>
       </c>
       <c r="N17">
-        <v>4.5521395752079037E-2</v>
+        <v>6.336093586561875E-2</v>
       </c>
       <c r="O17">
-        <v>0.70032722639946254</v>
+        <v>0.52417935966029816</v>
       </c>
       <c r="P17">
-        <v>1</v>
+        <v>0.99999999999998812</v>
       </c>
       <c r="Q17">
         <v>1</v>
       </c>
       <c r="R17">
-        <v>1.8287040964785031E-2</v>
+        <v>2.695617522830273E-2</v>
       </c>
       <c r="S17">
-        <v>4.4128596563195637E-3</v>
+        <v>6.2232389517752839E-4</v>
       </c>
       <c r="T17">
-        <v>7.7165038237553288E-2</v>
+        <v>2.813310267439862E-2</v>
       </c>
       <c r="U17">
-        <v>0.19096927518566811</v>
+        <v>8.6530265332053727E-2</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
@@ -1476,64 +1476,64 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="B18">
-        <v>2.1789919836982089E-4</v>
+        <v>1.4136308980620159E-3</v>
       </c>
       <c r="C18">
-        <v>7.4560962411704531E-3</v>
+        <v>1.3338649853724289E-4</v>
       </c>
       <c r="D18">
-        <v>8.7235605196196221E-4</v>
+        <v>9.9288215984399508E-4</v>
       </c>
       <c r="E18">
-        <v>2.4050491340163989E-8</v>
+        <v>8.1264830760232808E-8</v>
       </c>
       <c r="F18">
-        <v>3.3437872633855629E-8</v>
+        <v>3.3772957366291222E-8</v>
       </c>
       <c r="G18">
-        <v>4.3955822418248478E-11</v>
+        <v>1.9539623387759358E-12</v>
       </c>
       <c r="H18">
-        <v>2.5989928872761708E-4</v>
+        <v>5.0655873098462705E-4</v>
       </c>
       <c r="I18">
-        <v>6.198439090058077E-7</v>
+        <v>5.3539775809162536E-7</v>
       </c>
       <c r="J18">
-        <v>1.203136736078733E-3</v>
+        <v>5.1324067860262969E-4</v>
       </c>
       <c r="K18">
-        <v>3.609633144474376E-4</v>
+        <v>1.260346703722178E-3</v>
       </c>
       <c r="L18">
-        <v>1.2535561191343481E-3</v>
+        <v>1.530740753559435E-3</v>
       </c>
       <c r="M18">
-        <v>5.060755225612102E-7</v>
+        <v>7.2087879131648591E-7</v>
       </c>
       <c r="N18">
-        <v>3.7681179139172131E-5</v>
+        <v>5.187049399715414E-5</v>
       </c>
       <c r="O18">
-        <v>7.0361876474006636E-3</v>
+        <v>3.4789807213629008E-3</v>
       </c>
       <c r="P18">
-        <v>2.1403128583635481E-2</v>
+        <v>2.8133102674398051E-2</v>
       </c>
       <c r="Q18">
-        <v>1.8287040964785031E-2</v>
+        <v>2.695617522830273E-2</v>
       </c>
       <c r="R18">
         <v>1</v>
       </c>
       <c r="S18">
-        <v>0.67925868286976776</v>
+        <v>0.17397944400155399</v>
       </c>
       <c r="T18">
-        <v>0.51099388407113022</v>
+        <v>0.999999999999994</v>
       </c>
       <c r="U18">
-        <v>0.2427514843193217</v>
+        <v>0.62068557683642944</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
@@ -1541,64 +1541,64 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="B19">
-        <v>2.7845022154248019E-5</v>
+        <v>1.7102037483970849E-5</v>
       </c>
       <c r="C19">
-        <v>1.5826331585101429E-3</v>
+        <v>1.06107141825917E-6</v>
       </c>
       <c r="D19">
-        <v>1.5433898983535529E-4</v>
+        <v>1.392113014431501E-5</v>
       </c>
       <c r="E19">
-        <v>1.0558934461814369E-9</v>
+        <v>2.6247470567174799E-10</v>
       </c>
       <c r="F19">
-        <v>1.5173244844381209E-9</v>
+        <v>9.5239168603861024E-11</v>
       </c>
       <c r="G19">
-        <v>9.0292433946878349E-13</v>
+        <v>3.30014080024919E-15</v>
       </c>
       <c r="H19">
-        <v>3.2254242963141942E-5</v>
+        <v>4.3884573994100568E-6</v>
       </c>
       <c r="I19">
-        <v>3.5372785822630202E-8</v>
+        <v>1.648638884737745E-9</v>
       </c>
       <c r="J19">
-        <v>1.8654524256988891E-4</v>
+        <v>3.869742778490119E-6</v>
       </c>
       <c r="K19">
-        <v>4.5750780011298987E-5</v>
+        <v>1.230131765060612E-5</v>
       </c>
       <c r="L19">
-        <v>1.9729909762036189E-4</v>
+        <v>1.5472191632818931E-5</v>
       </c>
       <c r="M19">
-        <v>2.867621090557356E-8</v>
+        <v>2.787233900006273E-9</v>
       </c>
       <c r="N19">
-        <v>3.9468616145474359E-6</v>
+        <v>2.9946453924039251E-7</v>
       </c>
       <c r="O19">
-        <v>1.4576966258291451E-3</v>
+        <v>3.9052448377526308E-5</v>
       </c>
       <c r="P19">
-        <v>5.5588214737046938E-3</v>
+        <v>6.7728173313055795E-4</v>
       </c>
       <c r="Q19">
-        <v>4.4128596563195637E-3</v>
+        <v>6.2232389517752839E-4</v>
       </c>
       <c r="R19">
-        <v>0.67925868286976776</v>
+        <v>0.17397944400155399</v>
       </c>
       <c r="S19">
         <v>1</v>
       </c>
       <c r="T19">
-        <v>0.2706483718391503</v>
+        <v>0.17701342693064209</v>
       </c>
       <c r="U19">
-        <v>0.1012990711008981</v>
+        <v>6.8995290415880414E-2</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
@@ -1606,64 +1606,64 @@
         <v>1.9E-2</v>
       </c>
       <c r="B20">
-        <v>1.457696625829247E-3</v>
+        <v>1.5270157393455291E-3</v>
       </c>
       <c r="C20">
-        <v>3.510314829876366E-2</v>
+        <v>1.4844154560446441E-4</v>
       </c>
       <c r="D20">
-        <v>4.7798366882050164E-3</v>
+        <v>1.068054240261916E-3</v>
       </c>
       <c r="E20">
-        <v>2.4384086860006531E-7</v>
+        <v>1.003731476134684E-7</v>
       </c>
       <c r="F20">
-        <v>3.3681775712912058E-7</v>
+        <v>4.2560440834142919E-8</v>
       </c>
       <c r="G20">
-        <v>4.8043364493501045E-10</v>
+        <v>2.9135386384554079E-12</v>
       </c>
       <c r="H20">
-        <v>1.763703066628202E-3</v>
+        <v>5.5781136854532898E-4</v>
       </c>
       <c r="I20">
-        <v>5.9305609752617586E-6</v>
+        <v>6.5680099517370794E-7</v>
       </c>
       <c r="J20">
-        <v>7.1008947164402916E-3</v>
+        <v>5.6892603831093025E-4</v>
       </c>
       <c r="K20">
-        <v>2.4156140948717532E-3</v>
+        <v>1.3741641335705029E-3</v>
       </c>
       <c r="L20">
-        <v>7.3303458719044179E-3</v>
+        <v>1.664861959675016E-3</v>
       </c>
       <c r="M20">
-        <v>4.8478256205278986E-6</v>
+        <v>8.6450831582886772E-7</v>
       </c>
       <c r="N20">
-        <v>2.8139400653773121E-4</v>
+        <v>5.9057122000836537E-5</v>
       </c>
       <c r="O20">
-        <v>3.3690806688296292E-2</v>
+        <v>3.7517584822295241E-3</v>
       </c>
       <c r="P20">
-        <v>8.5526783091267961E-2</v>
+        <v>2.93262762513492E-2</v>
       </c>
       <c r="Q20">
-        <v>7.7165038237553288E-2</v>
+        <v>2.813310267439862E-2</v>
       </c>
       <c r="R20">
-        <v>0.51099388407113022</v>
+        <v>0.999999999999994</v>
       </c>
       <c r="S20">
-        <v>0.2706483718391503</v>
+        <v>0.17701342693064209</v>
       </c>
       <c r="T20">
         <v>1</v>
       </c>
       <c r="U20">
-        <v>0.60818217661565344</v>
+        <v>0.62336450632406215</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
@@ -1671,61 +1671,61 @@
         <v>0.02</v>
       </c>
       <c r="B21">
-        <v>5.2839601324109701E-3</v>
+        <v>6.6736722316070498E-3</v>
       </c>
       <c r="C21">
-        <v>9.5350640566264244E-2</v>
+        <v>8.2364487698628253E-4</v>
       </c>
       <c r="D21">
-        <v>1.492075737143009E-2</v>
+        <v>4.4959054682820734E-3</v>
       </c>
       <c r="E21">
-        <v>1.232362978881478E-6</v>
+        <v>1.0211313050519151E-6</v>
       </c>
       <c r="F21">
-        <v>1.694081506672887E-6</v>
+        <v>4.7622304855678139E-7</v>
       </c>
       <c r="G21">
-        <v>2.5293896648204482E-9</v>
+        <v>5.9786755238398405E-11</v>
       </c>
       <c r="H21">
-        <v>6.4407239952002414E-3</v>
+        <v>2.8590671473384252E-3</v>
       </c>
       <c r="I21">
-        <v>2.8607680003255519E-5</v>
+        <v>6.5242895106731733E-6</v>
       </c>
       <c r="J21">
-        <v>2.3125072238761819E-2</v>
+        <v>3.067918144626237E-3</v>
       </c>
       <c r="K21">
-        <v>8.7024165045004372E-3</v>
+        <v>6.5011712523409051E-3</v>
       </c>
       <c r="L21">
-        <v>2.371371235314473E-2</v>
+        <v>7.7149012146084774E-3</v>
       </c>
       <c r="M21">
-        <v>2.3418433924893479E-5</v>
+        <v>7.6034113311076567E-6</v>
       </c>
       <c r="N21">
-        <v>1.117803377350084E-3</v>
+        <v>3.8426256415280961E-4</v>
       </c>
       <c r="O21">
-        <v>9.2588237506403381E-2</v>
+        <v>1.6137422471564619E-2</v>
       </c>
       <c r="P21">
-        <v>0.2041556871143243</v>
+        <v>8.891860034689382E-2</v>
       </c>
       <c r="Q21">
-        <v>0.19096927518566811</v>
+        <v>8.6530265332053727E-2</v>
       </c>
       <c r="R21">
-        <v>0.2427514843193217</v>
+        <v>0.62068557683642944</v>
       </c>
       <c r="S21">
-        <v>0.1012990711008981</v>
+        <v>6.8995290415880414E-2</v>
       </c>
       <c r="T21">
-        <v>0.60818217661565344</v>
+        <v>0.62336450632406215</v>
       </c>
       <c r="U21">
         <v>1</v>
@@ -1733,12 +1733,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:U21">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="5"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color theme="0"/>
-        <color theme="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>